<commit_message>
fix error put file using form data
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">URLs</t>
   </si>
   <si>
-    <t xml:space="preserve">https://s3.amazonaws.com/static3.nft2scan.com/test/bnb-black.svg</t>
+    <t xml:space="preserve">https://s3.amazonaws.com/static3.nft2scan.com/test/nft1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://s3.amazonaws.com/static3.nft2scan.com/test/nft2.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://s3.amazonaws.com/static3.nft2scan.com/test/nft3.jpg</t>
   </si>
 </sst>
 </file>
@@ -35,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -71,6 +77,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -114,7 +126,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -124,6 +136,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,10 +167,10 @@
   <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="77.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.93"/>
@@ -166,15 +186,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
@@ -204,7 +224,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
@@ -572,9 +592,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://s3.amazonaws.com/static3.nft2scan.com/test/bnb-black.svg"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://s3.amazonaws.com/static3.nft2scan.com/test/bnb-black.svg"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://s3.amazonaws.com/static3.nft2scan.com/test/bnb-black.svg"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://s3.amazonaws.com/static3.nft2scan.com/test/nft1.jpg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>